<commit_message>
locators and object repository
</commit_message>
<xml_diff>
--- a/src/main/resources/locators/Locators.xlsx
+++ b/src/main/resources/locators/Locators.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>css</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Log In</t>
+  </si>
+  <si>
+    <t>input[class='btn'][value='Log In']</t>
   </si>
 </sst>
 </file>
@@ -483,7 +489,7 @@
   <dimension ref="A1:AT67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0"/>
@@ -570,7 +576,17 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="23" customHeight="1"/>
+    <row r="4" spans="1:46" ht="23" customHeight="1">
+      <c r="A4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
     <row r="5" spans="1:46" ht="23" customHeight="1"/>
     <row r="6" spans="1:46" ht="23" customHeight="1"/>
     <row r="7" spans="1:46" ht="23" customHeight="1"/>

</xml_diff>